<commit_message>
parameterized everying into a config.yaml now for scalability. also modularized and moved a lot of things to subfolders for better organization
</commit_message>
<xml_diff>
--- a/Publication/Outputs/Tables/ST1.xlsx
+++ b/Publication/Outputs/Tables/ST1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -47,81 +47,6 @@
     <t xml:space="preserve">949</t>
   </si>
   <si>
-    <t xml:space="preserve">  Multifocal Injury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">287 (31%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 (44%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.74 [0.89–3.42]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">303 (32%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Bilateral Injury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">245 (27%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (31%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.20 [0.58–2.47]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">256 (27%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Concomitant CBCVI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">154 (17%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (39%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.14 [1.57–6.27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">168 (18%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Median Grade (IQR)†</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 [1–3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 [2–4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ISS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 [10–29]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 [18–36]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  GCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 [11–15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 [5–15]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carotid</t>
   </si>
   <si>
@@ -132,75 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54 (14%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (20%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.54 [0.60–3.93]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 (14%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">138 (36%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (43%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.37 [0.65–2.91]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">151 (36%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Concomitant VBCVI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">154 (40%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (47%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.32 [0.63–2.78]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">168 (40%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 [1–2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 [1–4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5e-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 [21–41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34 [26–43]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 [22–41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 [3–15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 [3–14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.223</t>
   </si>
 </sst>
 </file>
@@ -583,255 +439,51 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D6"/>
       <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>